<commit_message>
Update 2022-09-11 #16 - Update Excel files.
</commit_message>
<xml_diff>
--- a/Excels/tha_adm_areas_adm1.xlsx
+++ b/Excels/tha_adm_areas_adm1.xlsx
@@ -1077,7 +1077,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1088,23 +1088,23 @@
   <dimension ref="A1:D78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.88671875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1115,10 +1115,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>30</v>
@@ -1129,10 +1129,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>42</v>
@@ -1143,10 +1143,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>72</v>
@@ -1157,10 +1157,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>224</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>225</v>
@@ -1171,10 +1171,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>120</v>
@@ -1185,10 +1185,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>215</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>216</v>
@@ -1199,10 +1199,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>149</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>150</v>
@@ -1213,10 +1213,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>123</v>
@@ -1227,10 +1227,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>45</v>
@@ -1241,10 +1241,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>108</v>
@@ -1255,10 +1255,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>153</v>
@@ -1269,10 +1269,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>48</v>
@@ -1283,10 +1283,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>200</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>201</v>
@@ -1297,10 +1297,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>230</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>231</v>
@@ -1311,10 +1311,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>60</v>
@@ -1325,10 +1325,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>183</v>
@@ -1339,10 +1339,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>162</v>
@@ -1353,10 +1353,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>75</v>
@@ -1367,10 +1367,10 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>117</v>
@@ -1381,10 +1381,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>176</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>177</v>
@@ -1395,10 +1395,10 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>6</v>
@@ -1409,10 +1409,10 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>114</v>
@@ -1423,10 +1423,10 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>189</v>
@@ -1437,10 +1437,10 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>206</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>207</v>
@@ -1451,10 +1451,10 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>111</v>
@@ -1465,10 +1465,10 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>90</v>
@@ -1479,10 +1479,10 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>209</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>210</v>
@@ -1493,10 +1493,10 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>93</v>
@@ -1507,10 +1507,10 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>167</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>168</v>
@@ -1521,10 +1521,10 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>57</v>
@@ -1535,10 +1535,10 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>135</v>
@@ -1549,10 +1549,10 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>18</v>
@@ -1563,10 +1563,10 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>96</v>
@@ -1577,10 +1577,10 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>191</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>192</v>
@@ -1591,10 +1591,10 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>165</v>
@@ -1605,10 +1605,10 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>212</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>213</v>
@@ -1619,10 +1619,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>141</v>
@@ -1633,10 +1633,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>9</v>
@@ -1647,10 +1647,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>227</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>228</v>
@@ -1661,10 +1661,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>69</v>
@@ -1675,10 +1675,10 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>54</v>
@@ -1689,10 +1689,10 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>197</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>198</v>
@@ -1703,10 +1703,10 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>170</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>171</v>
@@ -1717,10 +1717,10 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>129</v>
@@ -1731,10 +1731,10 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>87</v>
@@ -1745,10 +1745,10 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>27</v>
@@ -1759,10 +1759,10 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>185</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>186</v>
@@ -1773,10 +1773,10 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>233</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>234</v>
@@ -1787,10 +1787,10 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>174</v>
@@ -1801,10 +1801,10 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>63</v>
@@ -1815,10 +1815,10 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>221</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>222</v>
@@ -1829,10 +1829,10 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>39</v>
@@ -1843,10 +1843,10 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>144</v>
@@ -1857,10 +1857,10 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>21</v>
@@ -1871,10 +1871,10 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>84</v>
@@ -1885,10 +1885,10 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>24</v>
@@ -1899,10 +1899,10 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>194</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>195</v>
@@ -1913,10 +1913,10 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>33</v>
@@ -1927,10 +1927,10 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>36</v>
@@ -1941,10 +1941,10 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>180</v>
@@ -1955,10 +1955,10 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>203</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>204</v>
@@ -1969,10 +1969,10 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>102</v>
@@ -1983,10 +1983,10 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>132</v>
@@ -1997,10 +1997,10 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>99</v>
@@ -2011,10 +2011,10 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>158</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>159</v>
@@ -2025,10 +2025,10 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>147</v>
@@ -2039,10 +2039,10 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>66</v>
@@ -2053,10 +2053,10 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>12</v>
@@ -2067,10 +2067,10 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>218</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>219</v>
@@ -2081,10 +2081,10 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>78</v>
@@ -2095,10 +2095,10 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>81</v>
@@ -2109,10 +2109,10 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>51</v>
@@ -2123,10 +2123,10 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>138</v>
@@ -2137,10 +2137,10 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>126</v>
@@ -2151,10 +2151,10 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>155</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>156</v>
@@ -2165,10 +2165,10 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>15</v>
@@ -2179,10 +2179,10 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>105</v>

</xml_diff>